<commit_message>
do last save to be sure all is in
</commit_message>
<xml_diff>
--- a/ontology/dataset-voc.xlsx
+++ b/ontology/dataset-voc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jgraybeal/Documents/GitHub/fair-data-collective/generic-dataset-metadata-template/ontology/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75CA2940-922A-9C49-820A-3DADE7F1D514}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BA1C53D-6646-D84C-BE82-94DAD55ABE00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3440" yWindow="460" windowWidth="47040" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3557" uniqueCount="2386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3558" uniqueCount="2387">
   <si>
     <t>ConceptScheme URI</t>
   </si>
@@ -7297,9 +7297,6 @@
     <t>gdmt:MIMEType</t>
   </si>
   <si>
-    <t>2020-12-13T23:15:00-08:00</t>
-  </si>
-  <si>
     <t>Identifier Scheme</t>
   </si>
   <si>
@@ -7373,6 +7370,12 @@
   </si>
   <si>
     <t>application/x-bytecode.python</t>
+  </si>
+  <si>
+    <t>0.3.1</t>
+  </si>
+  <si>
+    <t>2020-12-13T23:45:00-08:00</t>
   </si>
 </sst>
 </file>
@@ -9354,8 +9357,8 @@
   <dimension ref="A1:W1157"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="187" workbookViewId="0">
-      <pane ySplit="16" topLeftCell="A999" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
+      <pane ySplit="16" topLeftCell="A687" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -9706,8 +9709,8 @@
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="2">
-        <v>0.3</v>
+      <c r="B12" s="2" t="s">
+        <v>2385</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -9765,7 +9768,7 @@
         <v>11</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>2375</v>
+        <v>2386</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
@@ -13175,7 +13178,7 @@
       <c r="C150" s="42"/>
       <c r="D150" s="42"/>
       <c r="E150" s="41" t="s">
-        <v>2377</v>
+        <v>2376</v>
       </c>
       <c r="F150" s="42"/>
       <c r="G150" s="42"/>
@@ -14596,7 +14599,7 @@
       <c r="C202" s="47"/>
       <c r="D202" s="47"/>
       <c r="E202" s="48" t="s">
-        <v>2378</v>
+        <v>2377</v>
       </c>
       <c r="F202" s="49"/>
       <c r="G202" s="49"/>
@@ -15104,7 +15107,7 @@
       <c r="C217" s="44"/>
       <c r="D217" s="44"/>
       <c r="E217" s="44" t="s">
-        <v>2379</v>
+        <v>2378</v>
       </c>
       <c r="F217" s="46"/>
       <c r="G217" s="46" t="s">
@@ -15172,7 +15175,7 @@
       <c r="C219" s="44"/>
       <c r="D219" s="44"/>
       <c r="E219" s="44" t="s">
-        <v>2380</v>
+        <v>2379</v>
       </c>
       <c r="F219" s="44"/>
       <c r="G219" s="46" t="s">
@@ -15342,7 +15345,7 @@
       <c r="C224" s="47"/>
       <c r="D224" s="47"/>
       <c r="E224" s="48" t="s">
-        <v>2381</v>
+        <v>2380</v>
       </c>
       <c r="F224" s="49"/>
       <c r="G224" s="49"/>
@@ -16627,7 +16630,7 @@
         <v>gdmt:IdentifierScheme</v>
       </c>
       <c r="B262" s="47" t="s">
-        <v>2376</v>
+        <v>2375</v>
       </c>
       <c r="C262" s="47"/>
       <c r="D262" s="47"/>
@@ -32241,7 +32244,7 @@
       <c r="C697" s="47"/>
       <c r="D697" s="47"/>
       <c r="E697" s="48" t="s">
-        <v>2382</v>
+        <v>2381</v>
       </c>
       <c r="F697" s="49"/>
       <c r="G697" s="49"/>
@@ -32307,7 +32310,7 @@
       <c r="C699" s="47"/>
       <c r="D699" s="47"/>
       <c r="E699" s="48" t="s">
-        <v>2383</v>
+        <v>2382</v>
       </c>
       <c r="F699" s="49"/>
       <c r="G699" s="49"/>
@@ -32372,7 +32375,7 @@
       <c r="C701" s="47"/>
       <c r="D701" s="47"/>
       <c r="E701" s="48" t="s">
-        <v>2384</v>
+        <v>2383</v>
       </c>
       <c r="F701" s="49"/>
       <c r="G701" s="49"/>
@@ -32399,7 +32402,7 @@
         <v>gdmt:application-x-bytecode.python</v>
       </c>
       <c r="B702" s="51" t="s">
-        <v>2385</v>
+        <v>2384</v>
       </c>
       <c r="C702" s="51"/>
       <c r="D702" s="51"/>

</xml_diff>

<commit_message>
updated with DataType properties
Replaced all appropriate rdf:type entries with DatatypeProperty
</commit_message>
<xml_diff>
--- a/ontology/dataset-voc.xlsx
+++ b/ontology/dataset-voc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Secondary_Drive/work/repos/FAIR-data/generic-dataset-metadata-template/ontology/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jgraybeal/Documents/GitHub/fair-data-collective/generic-dataset-metadata-template/ontology/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEBEFC53-DF34-7C48-A563-7A411389EA61}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B00DC0E-75E4-8E43-8BFB-0AB6752C4513}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34400" yWindow="460" windowWidth="34400" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3340" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="gdmt ontology" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3534" uniqueCount="2281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3534" uniqueCount="2282">
   <si>
     <t>ConceptScheme URI</t>
   </si>
@@ -7057,7 +7057,10 @@
     <t>0.3.3</t>
   </si>
   <si>
-    <t>2021-01-19T12:33:00+01:00</t>
+    <t>owl:DatatypeProperty</t>
+  </si>
+  <si>
+    <t>2021-01-19T20:29:00-08:00</t>
   </si>
 </sst>
 </file>
@@ -7361,7 +7364,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -7451,9 +7454,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="30" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -9039,8 +9039,8 @@
   <dimension ref="A1:W1147"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="187" workbookViewId="0">
-      <pane ySplit="16" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
+      <pane ySplit="16" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -9450,7 +9450,7 @@
         <v>11</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>2280</v>
+        <v>2281</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
@@ -10633,7 +10633,7 @@
         <v>2188</v>
       </c>
       <c r="C61" s="15" t="s">
-        <v>2041</v>
+        <v>2280</v>
       </c>
       <c r="D61" s="20" t="s">
         <v>2188</v>
@@ -10658,7 +10658,7 @@
         <v>2189</v>
       </c>
       <c r="C62" s="15" t="s">
-        <v>2041</v>
+        <v>2280</v>
       </c>
       <c r="D62" s="20" t="s">
         <v>2189</v>
@@ -10683,7 +10683,7 @@
         <v>2190</v>
       </c>
       <c r="C63" s="15" t="s">
-        <v>2041</v>
+        <v>2280</v>
       </c>
       <c r="D63" s="20" t="s">
         <v>2190</v>
@@ -10708,7 +10708,7 @@
         <v>2191</v>
       </c>
       <c r="C64" s="15" t="s">
-        <v>2041</v>
+        <v>2280</v>
       </c>
       <c r="D64" s="20" t="s">
         <v>2191</v>
@@ -10733,7 +10733,7 @@
         <v>2192</v>
       </c>
       <c r="C65" s="15" t="s">
-        <v>2041</v>
+        <v>2280</v>
       </c>
       <c r="D65" s="21" t="s">
         <v>2192</v>
@@ -10758,7 +10758,7 @@
         <v>2193</v>
       </c>
       <c r="C66" s="15" t="s">
-        <v>2041</v>
+        <v>2280</v>
       </c>
       <c r="D66" s="21" t="s">
         <v>2193</v>
@@ -10783,7 +10783,7 @@
         <v>2194</v>
       </c>
       <c r="C67" s="15" t="s">
-        <v>2041</v>
+        <v>2280</v>
       </c>
       <c r="D67" s="21" t="s">
         <v>2194</v>
@@ -10833,7 +10833,7 @@
         <v>2196</v>
       </c>
       <c r="C69" s="15" t="s">
-        <v>2041</v>
+        <v>2280</v>
       </c>
       <c r="D69" s="21" t="s">
         <v>2196</v>
@@ -10858,7 +10858,7 @@
         <v>2197</v>
       </c>
       <c r="C70" s="15" t="s">
-        <v>2041</v>
+        <v>2280</v>
       </c>
       <c r="D70" s="21" t="s">
         <v>2197</v>
@@ -10958,7 +10958,7 @@
         <v>2201</v>
       </c>
       <c r="C74" s="15" t="s">
-        <v>2041</v>
+        <v>2280</v>
       </c>
       <c r="D74" s="21" t="s">
         <v>2201</v>
@@ -10983,7 +10983,7 @@
         <v>2202</v>
       </c>
       <c r="C75" s="15" t="s">
-        <v>2041</v>
+        <v>2280</v>
       </c>
       <c r="D75" s="21" t="s">
         <v>2202</v>
@@ -11008,7 +11008,7 @@
         <v>2203</v>
       </c>
       <c r="C76" s="15" t="s">
-        <v>2041</v>
+        <v>2280</v>
       </c>
       <c r="D76" s="21" t="s">
         <v>2203</v>
@@ -11058,7 +11058,7 @@
         <v>2205</v>
       </c>
       <c r="C78" s="15" t="s">
-        <v>2041</v>
+        <v>2280</v>
       </c>
       <c r="D78" s="21" t="s">
         <v>2205</v>
@@ -11083,7 +11083,7 @@
         <v>2206</v>
       </c>
       <c r="C79" s="15" t="s">
-        <v>2041</v>
+        <v>2280</v>
       </c>
       <c r="D79" s="21" t="s">
         <v>2206</v>
@@ -11108,7 +11108,7 @@
         <v>2207</v>
       </c>
       <c r="C80" s="15" t="s">
-        <v>2041</v>
+        <v>2280</v>
       </c>
       <c r="D80" s="21" t="s">
         <v>2207</v>
@@ -11183,7 +11183,7 @@
         <v>2210</v>
       </c>
       <c r="C83" s="15" t="s">
-        <v>2041</v>
+        <v>2280</v>
       </c>
       <c r="D83" s="22" t="s">
         <v>2210</v>
@@ -11208,7 +11208,7 @@
         <v>2211</v>
       </c>
       <c r="C84" s="15" t="s">
-        <v>2041</v>
+        <v>2280</v>
       </c>
       <c r="D84" s="22" t="s">
         <v>2211</v>
@@ -11233,7 +11233,7 @@
         <v>2212</v>
       </c>
       <c r="C85" s="15" t="s">
-        <v>2041</v>
+        <v>2280</v>
       </c>
       <c r="D85" s="22" t="s">
         <v>2212</v>
@@ -11258,7 +11258,7 @@
         <v>2213</v>
       </c>
       <c r="C86" s="15" t="s">
-        <v>2041</v>
+        <v>2280</v>
       </c>
       <c r="D86" s="22" t="s">
         <v>2213</v>
@@ -11283,7 +11283,7 @@
         <v>2214</v>
       </c>
       <c r="C87" s="15" t="s">
-        <v>2041</v>
+        <v>2280</v>
       </c>
       <c r="D87" s="23" t="s">
         <v>2214</v>
@@ -11308,7 +11308,7 @@
         <v>2215</v>
       </c>
       <c r="C88" s="15" t="s">
-        <v>2041</v>
+        <v>2280</v>
       </c>
       <c r="D88" s="23" t="s">
         <v>2215</v>
@@ -11333,7 +11333,7 @@
         <v>2216</v>
       </c>
       <c r="C89" s="15" t="s">
-        <v>2041</v>
+        <v>2280</v>
       </c>
       <c r="D89" s="23" t="s">
         <v>2216</v>
@@ -11358,7 +11358,7 @@
         <v>2217</v>
       </c>
       <c r="C90" s="15" t="s">
-        <v>2041</v>
+        <v>2280</v>
       </c>
       <c r="D90" s="23" t="s">
         <v>2217</v>
@@ -11383,7 +11383,7 @@
         <v>2218</v>
       </c>
       <c r="C91" s="15" t="s">
-        <v>2041</v>
+        <v>2280</v>
       </c>
       <c r="D91" s="24" t="s">
         <v>2218</v>
@@ -11433,7 +11433,7 @@
         <v>2220</v>
       </c>
       <c r="C93" s="15" t="s">
-        <v>2041</v>
+        <v>2280</v>
       </c>
       <c r="D93" s="25" t="s">
         <v>2220</v>
@@ -11508,7 +11508,7 @@
         <v>2223</v>
       </c>
       <c r="C96" s="15" t="s">
-        <v>2041</v>
+        <v>2280</v>
       </c>
       <c r="D96" s="26" t="s">
         <v>2223</v>
@@ -11533,7 +11533,7 @@
         <v>2224</v>
       </c>
       <c r="C97" s="15" t="s">
-        <v>2041</v>
+        <v>2280</v>
       </c>
       <c r="D97" s="26" t="s">
         <v>2224</v>
@@ -11558,7 +11558,7 @@
         <v>2225</v>
       </c>
       <c r="C98" s="15" t="s">
-        <v>2041</v>
+        <v>2280</v>
       </c>
       <c r="D98" s="26" t="s">
         <v>2225</v>
@@ -11583,7 +11583,7 @@
         <v>2226</v>
       </c>
       <c r="C99" s="15" t="s">
-        <v>2041</v>
+        <v>2280</v>
       </c>
       <c r="D99" s="26" t="s">
         <v>2226</v>
@@ -11608,7 +11608,7 @@
         <v>2227</v>
       </c>
       <c r="C100" s="15" t="s">
-        <v>2041</v>
+        <v>2280</v>
       </c>
       <c r="D100" s="27" t="s">
         <v>2227</v>
@@ -11633,7 +11633,7 @@
         <v>2228</v>
       </c>
       <c r="C101" s="15" t="s">
-        <v>2041</v>
+        <v>2280</v>
       </c>
       <c r="D101" s="21" t="s">
         <v>2228</v>
@@ -11658,7 +11658,7 @@
         <v>2229</v>
       </c>
       <c r="C102" s="15" t="s">
-        <v>2041</v>
+        <v>2280</v>
       </c>
       <c r="D102" s="21" t="s">
         <v>2229</v>
@@ -11683,7 +11683,7 @@
         <v>2230</v>
       </c>
       <c r="C103" s="15" t="s">
-        <v>2041</v>
+        <v>2280</v>
       </c>
       <c r="D103" s="21" t="s">
         <v>2230</v>
@@ -11708,7 +11708,7 @@
         <v>2231</v>
       </c>
       <c r="C104" s="15" t="s">
-        <v>2041</v>
+        <v>2280</v>
       </c>
       <c r="D104" s="21" t="s">
         <v>2231</v>
@@ -11733,7 +11733,7 @@
         <v>2232</v>
       </c>
       <c r="C105" s="15" t="s">
-        <v>2041</v>
+        <v>2280</v>
       </c>
       <c r="D105" s="21" t="s">
         <v>2232</v>
@@ -11758,7 +11758,7 @@
         <v>2233</v>
       </c>
       <c r="C106" s="15" t="s">
-        <v>2041</v>
+        <v>2280</v>
       </c>
       <c r="D106" s="21" t="s">
         <v>2233</v>
@@ -11783,7 +11783,7 @@
         <v>2234</v>
       </c>
       <c r="C107" s="15" t="s">
-        <v>2041</v>
+        <v>2280</v>
       </c>
       <c r="D107" s="21" t="s">
         <v>2234</v>
@@ -11858,7 +11858,7 @@
         <v>2237</v>
       </c>
       <c r="C110" s="15" t="s">
-        <v>2041</v>
+        <v>2280</v>
       </c>
       <c r="D110" s="28" t="s">
         <v>2237</v>
@@ -11883,7 +11883,7 @@
         <v>2238</v>
       </c>
       <c r="C111" s="15" t="s">
-        <v>2041</v>
+        <v>2280</v>
       </c>
       <c r="D111" s="28" t="s">
         <v>2238</v>
@@ -11908,7 +11908,7 @@
         <v>2239</v>
       </c>
       <c r="C112" s="15" t="s">
-        <v>2041</v>
+        <v>2280</v>
       </c>
       <c r="D112" s="28" t="s">
         <v>2239</v>
@@ -11933,7 +11933,7 @@
         <v>2240</v>
       </c>
       <c r="C113" s="15" t="s">
-        <v>2041</v>
+        <v>2280</v>
       </c>
       <c r="D113" s="28" t="s">
         <v>2240</v>
@@ -11958,7 +11958,7 @@
         <v>2241</v>
       </c>
       <c r="C114" s="15" t="s">
-        <v>2041</v>
+        <v>2280</v>
       </c>
       <c r="D114" s="28" t="s">
         <v>2241</v>
@@ -11983,7 +11983,7 @@
         <v>2242</v>
       </c>
       <c r="C115" s="15" t="s">
-        <v>2041</v>
+        <v>2280</v>
       </c>
       <c r="D115" s="28" t="s">
         <v>2242</v>
@@ -12008,7 +12008,7 @@
         <v>2243</v>
       </c>
       <c r="C116" s="15" t="s">
-        <v>2041</v>
+        <v>2280</v>
       </c>
       <c r="D116" s="28" t="s">
         <v>2243</v>
@@ -12033,7 +12033,7 @@
         <v>2244</v>
       </c>
       <c r="C117" s="15" t="s">
-        <v>2041</v>
+        <v>2280</v>
       </c>
       <c r="D117" s="28" t="s">
         <v>2244</v>
@@ -12058,7 +12058,7 @@
         <v>2245</v>
       </c>
       <c r="C118" s="15" t="s">
-        <v>2041</v>
+        <v>2280</v>
       </c>
       <c r="D118" s="28" t="s">
         <v>2245</v>
@@ -12083,7 +12083,7 @@
         <v>2246</v>
       </c>
       <c r="C119" s="15" t="s">
-        <v>2041</v>
+        <v>2280</v>
       </c>
       <c r="D119" s="28" t="s">
         <v>2246</v>
@@ -12108,7 +12108,7 @@
         <v>2247</v>
       </c>
       <c r="C120" s="15" t="s">
-        <v>2041</v>
+        <v>2280</v>
       </c>
       <c r="D120" s="28" t="s">
         <v>2247</v>
@@ -12133,7 +12133,7 @@
         <v>2248</v>
       </c>
       <c r="C121" s="15" t="s">
-        <v>2041</v>
+        <v>2280</v>
       </c>
       <c r="D121" s="28" t="s">
         <v>2248</v>
@@ -12158,7 +12158,7 @@
         <v>2249</v>
       </c>
       <c r="C122" s="15" t="s">
-        <v>2041</v>
+        <v>2280</v>
       </c>
       <c r="D122" s="29" t="s">
         <v>2249</v>
@@ -12183,7 +12183,7 @@
         <v>2250</v>
       </c>
       <c r="C123" s="15" t="s">
-        <v>2041</v>
+        <v>2280</v>
       </c>
       <c r="D123" s="29" t="s">
         <v>2250</v>
@@ -12208,7 +12208,7 @@
         <v>2251</v>
       </c>
       <c r="C124" s="15" t="s">
-        <v>2041</v>
+        <v>2280</v>
       </c>
       <c r="D124" s="25" t="s">
         <v>2251</v>
@@ -12233,7 +12233,7 @@
         <v>2252</v>
       </c>
       <c r="C125" s="15" t="s">
-        <v>2041</v>
+        <v>2280</v>
       </c>
       <c r="D125" s="25" t="s">
         <v>2252</v>
@@ -12258,7 +12258,7 @@
         <v>2253</v>
       </c>
       <c r="C126" s="15" t="s">
-        <v>2041</v>
+        <v>2280</v>
       </c>
       <c r="D126" s="25" t="s">
         <v>2253</v>
@@ -12283,7 +12283,7 @@
         <v>2254</v>
       </c>
       <c r="C127" s="15" t="s">
-        <v>2041</v>
+        <v>2280</v>
       </c>
       <c r="D127" s="25" t="s">
         <v>2254</v>
@@ -12308,7 +12308,7 @@
         <v>2255</v>
       </c>
       <c r="C128" s="15" t="s">
-        <v>2041</v>
+        <v>2280</v>
       </c>
       <c r="D128" s="29" t="s">
         <v>2255</v>
@@ -12333,7 +12333,7 @@
         <v>2256</v>
       </c>
       <c r="C129" s="15" t="s">
-        <v>2041</v>
+        <v>2280</v>
       </c>
       <c r="D129" s="29" t="s">
         <v>2256</v>
@@ -12358,7 +12358,7 @@
         <v>2257</v>
       </c>
       <c r="C130" s="15" t="s">
-        <v>2041</v>
+        <v>2280</v>
       </c>
       <c r="D130" s="25" t="s">
         <v>2257</v>
@@ -12383,7 +12383,7 @@
         <v>2258</v>
       </c>
       <c r="C131" s="15" t="s">
-        <v>2041</v>
+        <v>2280</v>
       </c>
       <c r="D131" s="30" t="s">
         <v>2258</v>
@@ -12408,7 +12408,7 @@
         <v>2259</v>
       </c>
       <c r="C132" s="15" t="s">
-        <v>2041</v>
+        <v>2280</v>
       </c>
       <c r="D132" s="30" t="s">
         <v>2259</v>
@@ -12458,7 +12458,7 @@
         <v>2261</v>
       </c>
       <c r="C134" s="15" t="s">
-        <v>2041</v>
+        <v>2280</v>
       </c>
       <c r="D134" s="30" t="s">
         <v>2261</v>
@@ -12482,8 +12482,8 @@
       <c r="B135" s="30" t="s">
         <v>2262</v>
       </c>
-      <c r="C135" s="54" t="s">
-        <v>2041</v>
+      <c r="C135" s="15" t="s">
+        <v>2280</v>
       </c>
       <c r="D135" s="30" t="s">
         <v>2262</v>
@@ -12508,7 +12508,7 @@
         <v>2263</v>
       </c>
       <c r="C136" s="15" t="s">
-        <v>2041</v>
+        <v>2280</v>
       </c>
       <c r="D136" s="30" t="s">
         <v>2263</v>
@@ -12532,8 +12532,8 @@
       <c r="B137" s="30" t="s">
         <v>2264</v>
       </c>
-      <c r="C137" s="54" t="s">
-        <v>2041</v>
+      <c r="C137" s="15" t="s">
+        <v>2280</v>
       </c>
       <c r="D137" s="30" t="s">
         <v>2264</v>
@@ -12558,7 +12558,7 @@
         <v>2265</v>
       </c>
       <c r="C138" s="15" t="s">
-        <v>2041</v>
+        <v>2280</v>
       </c>
       <c r="D138" s="30" t="s">
         <v>2265</v>
@@ -12582,8 +12582,8 @@
       <c r="B139" s="31" t="s">
         <v>2266</v>
       </c>
-      <c r="C139" s="54" t="s">
-        <v>2041</v>
+      <c r="C139" s="15" t="s">
+        <v>2280</v>
       </c>
       <c r="D139" s="31" t="s">
         <v>2266</v>
@@ -12607,8 +12607,8 @@
       <c r="B140" s="31" t="s">
         <v>2267</v>
       </c>
-      <c r="C140" s="54" t="s">
-        <v>2041</v>
+      <c r="C140" s="15" t="s">
+        <v>2280</v>
       </c>
       <c r="D140" s="31" t="s">
         <v>2267</v>
@@ -12633,7 +12633,7 @@
         <v>2268</v>
       </c>
       <c r="C141" s="15" t="s">
-        <v>2041</v>
+        <v>2280</v>
       </c>
       <c r="D141" s="31" t="s">
         <v>2268</v>
@@ -12657,8 +12657,8 @@
       <c r="B142" s="31" t="s">
         <v>2269</v>
       </c>
-      <c r="C142" s="54" t="s">
-        <v>2041</v>
+      <c r="C142" s="15" t="s">
+        <v>2280</v>
       </c>
       <c r="D142" s="31" t="s">
         <v>2269</v>
@@ -12682,8 +12682,8 @@
       <c r="B143" s="32" t="s">
         <v>2270</v>
       </c>
-      <c r="C143" s="54" t="s">
-        <v>2041</v>
+      <c r="C143" s="15" t="s">
+        <v>2280</v>
       </c>
       <c r="D143" s="32" t="s">
         <v>2270</v>
@@ -12707,8 +12707,8 @@
       <c r="B144" s="32" t="s">
         <v>2271</v>
       </c>
-      <c r="C144" s="54" t="s">
-        <v>2041</v>
+      <c r="C144" s="15" t="s">
+        <v>2280</v>
       </c>
       <c r="D144" s="32" t="s">
         <v>2271</v>
@@ -12732,8 +12732,8 @@
       <c r="B145" s="32" t="s">
         <v>2272</v>
       </c>
-      <c r="C145" s="54" t="s">
-        <v>2041</v>
+      <c r="C145" s="15" t="s">
+        <v>2280</v>
       </c>
       <c r="D145" s="32" t="s">
         <v>2272</v>
@@ -12757,8 +12757,8 @@
       <c r="B146" s="32" t="s">
         <v>2273</v>
       </c>
-      <c r="C146" s="54" t="s">
-        <v>2041</v>
+      <c r="C146" s="15" t="s">
+        <v>2280</v>
       </c>
       <c r="D146" s="32" t="s">
         <v>2273</v>
@@ -12783,7 +12783,7 @@
         <v>2274</v>
       </c>
       <c r="C147" s="15" t="s">
-        <v>2041</v>
+        <v>2280</v>
       </c>
       <c r="D147" s="32" t="s">
         <v>2274</v>
@@ -12807,8 +12807,8 @@
       <c r="B148" s="32" t="s">
         <v>2275</v>
       </c>
-      <c r="C148" s="54" t="s">
-        <v>2041</v>
+      <c r="C148" s="15" t="s">
+        <v>2280</v>
       </c>
       <c r="D148" s="32" t="s">
         <v>2275</v>
@@ -12833,7 +12833,7 @@
         <v>2276</v>
       </c>
       <c r="C149" s="15" t="s">
-        <v>2041</v>
+        <v>2280</v>
       </c>
       <c r="D149" s="32" t="s">
         <v>2276</v>

</xml_diff>